<commit_message>
feat: Add script to unify teams with name changes and consolidate player statistics
- Implemented a Python script to rename team references and consolidate statistics for players affected by team name changes.
- Added functionality to backup data before processing.
- Included logging for tracking changes and processing status.
- Consolidated duplicate players and teams based on specified criteria.
- Supported processing of Excel files containing team and player data.
</commit_message>
<xml_diff>
--- a/data/2FEB_25_26/players_25_26_2FEB.xlsx
+++ b/data/2FEB_25_26/players_25_26_2FEB.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>JUGADOR</t>
+          <t>JUGADOR.1</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -15880,7 +15880,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G168" t="n">
@@ -15973,7 +15973,7 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G169" t="n">
@@ -16066,7 +16066,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G170" t="n">
@@ -16159,7 +16159,7 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G171" t="n">
@@ -16499,7 +16499,7 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G175" t="n">
@@ -16592,7 +16592,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G176" t="n">
@@ -16685,7 +16685,7 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G177" t="n">
@@ -16778,7 +16778,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G178" t="n">
@@ -16871,7 +16871,7 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>UEMC CBC VALLADOLID</t>
+          <t>UEMC BALONCESTO VALLADOLID</t>
         </is>
       </c>
       <c r="G179" t="n">

</xml_diff>